<commit_message>
pulled archives back for small models
</commit_message>
<xml_diff>
--- a/prompts_benchmarks.xlsx
+++ b/prompts_benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/code/digitalsynergy/ollama-prompts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5FDC0-C921-5645-B163-E9FCCC09A816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B734FFD7-D867-624F-9F66-4817DEE5F955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="1320" windowWidth="25800" windowHeight="16940" xr2:uid="{9C1B02D5-A4F4-2B4F-972D-1C4731664FEF}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="2000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3292" uniqueCount="2201">
   <si>
     <t>Magic 8-Ball - Sonnet</t>
   </si>
@@ -9051,6 +9051,609 @@
   </si>
   <si>
     <t>there are 48 students on the soccer team.</t>
+  </si>
+  <si>
+    <t>9907B854-0F36-4B18-8F4B-8334F00C48B7</t>
+  </si>
+  <si>
+    <t>🩺</t>
+  </si>
+  <si>
+    <t>Medical and Health Advice</t>
+  </si>
+  <si>
+    <t>Explain the potential benefits and risks of intermittent fasting for weight loss.</t>
+  </si>
+  <si>
+    <t>76E90DE9-66D5-4EEE-9C5D-3763C99699D9</t>
+  </si>
+  <si>
+    <t>What are the common symptoms and early warning signs of type 2 diabetes?</t>
+  </si>
+  <si>
+    <t>12822FFD-C39D-415D-87EB-1377F2639CD6</t>
+  </si>
+  <si>
+    <t>How can someone manage chronic pain without relying heavily on medication?</t>
+  </si>
+  <si>
+    <t>A8D92F33-865D-4776-A380-1137C665CAA2</t>
+  </si>
+  <si>
+    <t>What are the best dietary practices for maintaining heart health in individuals over 50?</t>
+  </si>
+  <si>
+    <t>64312FCA-BD73-4A8C-9DC9-8DAAA09F22E2</t>
+  </si>
+  <si>
+    <t>How does regular physical exercise impact mental health and cognitive function?</t>
+  </si>
+  <si>
+    <t>54D836CD-0186-4994-A75A-060F331870D2</t>
+  </si>
+  <si>
+    <t>What are the latest advancements in treating autoimmune diseases?</t>
+  </si>
+  <si>
+    <t>634B0B24-F61A-44BD-B613-1BF1A1867466</t>
+  </si>
+  <si>
+    <t>Explain the role of gut microbiome in overall health and its connection to mental well-being.</t>
+  </si>
+  <si>
+    <t>7BED3125-17EF-4DA9-976A-3EFA43A2D295</t>
+  </si>
+  <si>
+    <t>What lifestyle changes can help reduce the risk of developing osteoporosis?</t>
+  </si>
+  <si>
+    <t>565C9DD4-F7EB-4D04-AE01-43B4E06FFD36</t>
+  </si>
+  <si>
+    <t>How does smoking affect lung health, and what are effective strategies for quitting?</t>
+  </si>
+  <si>
+    <t>8D98B0A9-7DC3-4265-A5DA-9E0FD19255ED</t>
+  </si>
+  <si>
+    <t>What are the risks and benefits of using telemedicine for regular health check-ups?</t>
+  </si>
+  <si>
+    <t>E6E8AD2A-6188-404B-A5AC-CE4B7A1425BA</t>
+  </si>
+  <si>
+    <t>🧠</t>
+  </si>
+  <si>
+    <t>Psychology and Human Behavior</t>
+  </si>
+  <si>
+    <t>How can one cultivate emotional resilience in the face of personal challenges?</t>
+  </si>
+  <si>
+    <t>C5F41B93-EFFE-4D24-B89C-CFCD82441AF3</t>
+  </si>
+  <si>
+    <t>What are effective strategies for managing anxiety in high-stress situations?</t>
+  </si>
+  <si>
+    <t>71FE7DE2-FDE6-4D9A-9185-CD049E1C5797</t>
+  </si>
+  <si>
+    <t>How does cognitive-behavioral therapy help in changing negative thought patterns?</t>
+  </si>
+  <si>
+    <t>ECC8F751-6D14-4A1C-9841-649B0932E5AA</t>
+  </si>
+  <si>
+    <t>What role does mindfulness play in improving mental health and well-being?</t>
+  </si>
+  <si>
+    <t>DAC7B050-C6F6-4269-8C43-150B798F0063</t>
+  </si>
+  <si>
+    <t>How can someone develop healthier coping mechanisms for dealing with grief?</t>
+  </si>
+  <si>
+    <t>4FE856B5-952D-44CC-8E70-0ADAFBC575B6</t>
+  </si>
+  <si>
+    <t>Explain the connection between sleep quality and mental health.</t>
+  </si>
+  <si>
+    <t>D7D58607-B0F4-475C-9FE1-DE4EDAD5DA33</t>
+  </si>
+  <si>
+    <t>What are the most common signs of burnout, and how can it be prevented?</t>
+  </si>
+  <si>
+    <t>D2871F46-C962-4858-AA61-BC8C236A8EDA</t>
+  </si>
+  <si>
+    <t>How can someone practice self-compassion in their daily life?</t>
+  </si>
+  <si>
+    <t>7ADCCC46-2791-4C09-A227-7B3733065A5C</t>
+  </si>
+  <si>
+    <t>What are the benefits of journaling for mental health?</t>
+  </si>
+  <si>
+    <t>ED4D0943-03BB-4C7C-8E8B-9C2C58A0882B</t>
+  </si>
+  <si>
+    <t>How can one overcome the fear of failure and embrace growth?</t>
+  </si>
+  <si>
+    <t>80A0A11F-0C0A-4813-8755-E571A06A1349</t>
+  </si>
+  <si>
+    <t>📊</t>
+  </si>
+  <si>
+    <t>Business Strategy and Financial Analysis</t>
+  </si>
+  <si>
+    <t>How can a company effectively pivot its business model in response to market disruptions?</t>
+  </si>
+  <si>
+    <t>0374DEC4-73CA-487B-AF7A-4B7FCB5EAE94</t>
+  </si>
+  <si>
+    <t>What are the key financial ratios to evaluate the health of a business?</t>
+  </si>
+  <si>
+    <t>7B1059CC-F6A8-42DC-A960-56521C95D8D5</t>
+  </si>
+  <si>
+    <t>How does competitive analysis influence a company's strategic planning?</t>
+  </si>
+  <si>
+    <t>B558FD8E-564E-41F1-B06F-EA6EDD4530A5</t>
+  </si>
+  <si>
+    <t>What strategies can a business use to improve its profit margins?</t>
+  </si>
+  <si>
+    <t>8C102F2E-25C2-4789-BD00-D2D9E68450A2</t>
+  </si>
+  <si>
+    <t>Explain the importance of cash flow management in business sustainability.</t>
+  </si>
+  <si>
+    <t>4B6FED52-7D26-44DF-BA96-604DA01B169E</t>
+  </si>
+  <si>
+    <t>How can a company optimize its supply chain to reduce costs and increase efficiency?</t>
+  </si>
+  <si>
+    <t>E317BDDF-EFAF-43A6-BCFB-E51CB4E1A868</t>
+  </si>
+  <si>
+    <t>What role does customer segmentation play in developing a successful marketing strategy?</t>
+  </si>
+  <si>
+    <t>AF323E48-66E5-4C04-A80B-1EAC3CFB9293</t>
+  </si>
+  <si>
+    <t>How should a business evaluate the risk versus reward of entering a new market?</t>
+  </si>
+  <si>
+    <t>1361E0A9-EBC4-47D5-B684-53DD43E45744</t>
+  </si>
+  <si>
+    <t>What are effective strategies for managing business debt?</t>
+  </si>
+  <si>
+    <t>780D0379-064F-47FD-BFFE-34453DD2B5FF</t>
+  </si>
+  <si>
+    <t>How can a company leverage technology to gain a competitive advantage?</t>
+  </si>
+  <si>
+    <t>625EDFC9-120C-472B-9F2D-AA06DC6D52F9</t>
+  </si>
+  <si>
+    <t>🖌️</t>
+  </si>
+  <si>
+    <t>User Interface and UX Design</t>
+  </si>
+  <si>
+    <t>How can user research inform the design of a more intuitive user interface?</t>
+  </si>
+  <si>
+    <t>7C42D729-470D-4DDC-A05B-5A2FE77916B1</t>
+  </si>
+  <si>
+    <t>What are the best practices for designing accessible user interfaces for people with disabilities?</t>
+  </si>
+  <si>
+    <t>124C7536-2936-4BD3-B1F2-0EA84597BE72</t>
+  </si>
+  <si>
+    <t>How does the choice of color scheme impact user experience in an application?</t>
+  </si>
+  <si>
+    <t>14D0BFB3-6154-4CC7-9817-4074A020544C</t>
+  </si>
+  <si>
+    <t>What techniques can be used to improve the usability of a complex form or workflow?</t>
+  </si>
+  <si>
+    <t>60994FA6-8DAF-497C-BF9B-FAFABF46FC7E</t>
+  </si>
+  <si>
+    <t>How can microinteractions enhance the overall user experience?</t>
+  </si>
+  <si>
+    <t>EA6162F9-CE62-40CC-838D-F77BED0D6463</t>
+  </si>
+  <si>
+    <t>What role does consistency play in UI/UX design across multiple platforms?</t>
+  </si>
+  <si>
+    <t>F7AD9C22-2633-4B43-B9CE-5B151556F02D</t>
+  </si>
+  <si>
+    <t>How should a designer approach creating a mobile-first user interface?</t>
+  </si>
+  <si>
+    <t>2125B0AC-DADC-402C-B71E-11663D1EA3C9</t>
+  </si>
+  <si>
+    <t>What are effective methods for conducting usability testing on a new design?</t>
+  </si>
+  <si>
+    <t>E4EC76BF-E893-4C39-BF6F-246B0E290363</t>
+  </si>
+  <si>
+    <t>How can animation be used to guide users and improve navigation in an app?</t>
+  </si>
+  <si>
+    <t>9306B5D9-D998-465E-8EED-0270B3F223FC</t>
+  </si>
+  <si>
+    <t>What strategies can be employed to reduce user cognitive load in an interface?</t>
+  </si>
+  <si>
+    <t>FFCBE1A5-2CB5-4413-BE0F-C91C1EFE364C</t>
+  </si>
+  <si>
+    <t>🌍</t>
+  </si>
+  <si>
+    <t>Environmental Science and Sustainability</t>
+  </si>
+  <si>
+    <t>How can renewable energy sources be integrated into existing power grids to reduce reliance on fossil fuels?</t>
+  </si>
+  <si>
+    <t>06C53B45-8416-458B-B793-CDD2C20FA1F3</t>
+  </si>
+  <si>
+    <t>What are the most effective strategies for mitigating the impacts of climate change on coastal communities?</t>
+  </si>
+  <si>
+    <t>7AC7DB93-DA1A-4503-9F38-C53398390F7F</t>
+  </si>
+  <si>
+    <t>How does deforestation affect biodiversity and what can be done to prevent it?</t>
+  </si>
+  <si>
+    <t>E0458AA2-B952-49A7-9F45-72634C88D690</t>
+  </si>
+  <si>
+    <t>What are the potential benefits and drawbacks of geoengineering as a solution to climate change?</t>
+  </si>
+  <si>
+    <t>4B14AA29-54C2-4643-8454-2F4898A375A1</t>
+  </si>
+  <si>
+    <t>How can urban planning be optimized to promote sustainability and reduce environmental footprints?</t>
+  </si>
+  <si>
+    <t>B1800FA4-1E10-47F5-8C70-F10FB6ACAFD6</t>
+  </si>
+  <si>
+    <t>What role do wetlands play in carbon sequestration and how can they be protected?</t>
+  </si>
+  <si>
+    <t>079E1D06-E458-45AC-A2C5-95725B0C3BE1</t>
+  </si>
+  <si>
+    <t>How can the circular economy model be implemented to minimize waste in manufacturing industries?</t>
+  </si>
+  <si>
+    <t>38EA42C8-4092-4101-A9EA-530A58A25A53</t>
+  </si>
+  <si>
+    <t>What are the challenges and solutions for managing plastic pollution in oceans and waterways?</t>
+  </si>
+  <si>
+    <t>AF3B3D41-E9BE-4A12-A83B-CAF6B171ADB7</t>
+  </si>
+  <si>
+    <t>How can agricultural practices be improved to enhance soil health and reduce the need for chemical inputs?</t>
+  </si>
+  <si>
+    <t>B7AA925A-05A2-4AD2-8205-127C279910AC</t>
+  </si>
+  <si>
+    <t>What are the most promising technologies for capturing and storing carbon emissions?</t>
+  </si>
+  <si>
+    <t>0B609E8A-AB2A-46BC-8E7F-EAF38367AB90</t>
+  </si>
+  <si>
+    <t>📈</t>
+  </si>
+  <si>
+    <t>Project Management and Agile Methodologies</t>
+  </si>
+  <si>
+    <t>How can the principles of Agile methodology improve team collaboration and project delivery?</t>
+  </si>
+  <si>
+    <t>51D01FFC-EB30-4740-BD01-D8617379753E</t>
+  </si>
+  <si>
+    <t>What are the key differences between Scrum and Kanban in Agile project management?</t>
+  </si>
+  <si>
+    <t>BCF42B72-D65D-480B-921C-A55A3282BA3D</t>
+  </si>
+  <si>
+    <t>How can project managers effectively manage scope creep in Agile projects?</t>
+  </si>
+  <si>
+    <t>7719BC2E-EBD6-49F0-A790-8FDF4EF49268</t>
+  </si>
+  <si>
+    <t>What are the best practices for conducting effective Agile retrospectives?</t>
+  </si>
+  <si>
+    <t>A60553C5-EBDE-4E5B-9E04-9933D35D9DE4</t>
+  </si>
+  <si>
+    <t>How can Lean methodology be applied to reduce waste and increase efficiency in project management?</t>
+  </si>
+  <si>
+    <t>2ED6A036-CF2A-4739-9EFF-B554E541D790</t>
+  </si>
+  <si>
+    <t>What are the most common challenges faced when transitioning to Agile methodologies, and how can they be overcome?</t>
+  </si>
+  <si>
+    <t>48BFE0C4-B279-4C07-A9F2-7C35D289696D</t>
+  </si>
+  <si>
+    <t>How can Lean thinking be integrated with Agile practices to optimize value delivery?</t>
+  </si>
+  <si>
+    <t>B8F15974-58AC-48FF-B1B3-77FD41985E6D</t>
+  </si>
+  <si>
+    <t>What strategies can be used to maintain team motivation and productivity in long-running Agile projects?</t>
+  </si>
+  <si>
+    <t>995D88D0-DCD2-4CCB-B4EF-AB215587AFE6</t>
+  </si>
+  <si>
+    <t>How can Agile project management be scaled across large, distributed teams?</t>
+  </si>
+  <si>
+    <t>16888405-E74E-43B6-9B77-D1E0E1607EBC</t>
+  </si>
+  <si>
+    <t>What are the key metrics for measuring the success of Agile projects?</t>
+  </si>
+  <si>
+    <t>3EDDDC27-E9F9-4514-B0EE-3C1369033442</t>
+  </si>
+  <si>
+    <t>📜</t>
+  </si>
+  <si>
+    <t>Alternative Histories</t>
+  </si>
+  <si>
+    <t>Imagine a world where the Roman Empire never fell and write a short story about how society would function today under its rule. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>C76BCB67-C3B2-43FB-BD43-D56249B5B1C7</t>
+  </si>
+  <si>
+    <t>Write a short story about an alternate history where the printing press was never invented and its impact on global knowledge and power structures. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>210E6747-5A83-4842-9876-73FFF4C4BFB5</t>
+  </si>
+  <si>
+    <t>Create a short story where Nikola Tesla's wireless energy technology became the dominant global power source in the early 20th century. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>14A5C592-44DE-43C0-A5B8-43DC55E56502</t>
+  </si>
+  <si>
+    <t>Write a short story about a world where the American Revolution failed and the United States remained under British control. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>3B47C6DB-F0BD-48E1-8D25-5F4816C68DE1</t>
+  </si>
+  <si>
+    <t>Imagine a world where World War I never happened and explore the societal and technological advances of the 20th century in a short story. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>90C9B1F0-0972-4428-8FF5-EC6B3650D2CC</t>
+  </si>
+  <si>
+    <t>Write a short story where ancient civilizations like the Mayans or Egyptians discovered space travel and explored the cosmos. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>4A156D53-8138-4C3F-ACC7-91DED78AC66D</t>
+  </si>
+  <si>
+    <t>Create a short story about an alternate history where the internet was invented in the 19th century during the Industrial Revolution. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>4B4E0401-05F8-4EC4-8DA3-3687B8A50CAB</t>
+  </si>
+  <si>
+    <t>Imagine a world where the Soviet Union won the Cold War and became the dominant global superpower. Write a short story exploring the cultural and political landscape. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>F1B04E95-3555-49F4-B314-78E473A742FA</t>
+  </si>
+  <si>
+    <t>Write a short story about an alternate history where the Black Death never occurred, and Europe never experienced the Renaissance. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>C764017F-0C23-4C20-9A56-32BEFB88C153</t>
+  </si>
+  <si>
+    <t>Create a short story where the abolition of slavery never happened, and explore the impact on modern society. (Under 1000 words)</t>
+  </si>
+  <si>
+    <t>2348A31E-58F8-4CBC-8066-B81D1124F965</t>
+  </si>
+  <si>
+    <t>💼</t>
+  </si>
+  <si>
+    <t>Economic Theories and Policy Analysis</t>
+  </si>
+  <si>
+    <t>Explain the potential impact of a universal basic income on global economies, considering both positive and negative effects.</t>
+  </si>
+  <si>
+    <t>334AC845-E2BF-46D9-A202-D28C97DEE2BB</t>
+  </si>
+  <si>
+    <t>Analyze the effects of implementing a flat tax rate in a developed economy, including possible changes in income distribution and government revenue.</t>
+  </si>
+  <si>
+    <t>96CA15C6-B98B-4882-B80F-6C9BCCA8A513</t>
+  </si>
+  <si>
+    <t>Discuss how Keynesian economic theory would address a modern-day economic recession caused by a global pandemic.</t>
+  </si>
+  <si>
+    <t>C7879490-5800-4652-9F54-4B4519BDF1B1</t>
+  </si>
+  <si>
+    <t>Compare and contrast the outcomes of supply-side economics versus demand-side economics in boosting economic growth.</t>
+  </si>
+  <si>
+    <t>190D4186-27D3-4452-8983-956D87C7C680</t>
+  </si>
+  <si>
+    <t>Examine the potential consequences of adopting Modern Monetary Theory (MMT) in a country with high national debt.</t>
+  </si>
+  <si>
+    <t>89A2071E-D30F-414F-96E6-2B4D7BF17DB5</t>
+  </si>
+  <si>
+    <t>Analyze the long-term economic impact of protectionist trade policies on both domestic industries and global markets.</t>
+  </si>
+  <si>
+    <t>EAB56912-065E-41D8-9215-7EC369778342</t>
+  </si>
+  <si>
+    <t>Discuss the role of central banks in managing inflation and maintaining economic stability in a post-pandemic world.</t>
+  </si>
+  <si>
+    <t>A19AA6BA-EFF1-4169-8E8C-12CD01C7B514</t>
+  </si>
+  <si>
+    <t>Evaluate the effectiveness of austerity measures in reducing national debt and their impact on social welfare programs.</t>
+  </si>
+  <si>
+    <t>18F01E0F-3FBC-4D43-8ECE-768617691178</t>
+  </si>
+  <si>
+    <t>Explore the relationship between economic inequality and political instability, using historical and contemporary examples.</t>
+  </si>
+  <si>
+    <t>C82EB8FA-017B-4565-8448-34A68E9B9D8C</t>
+  </si>
+  <si>
+    <t>Analyze the potential effects of a carbon tax on both the economy and the environment, considering short-term and long-term outcomes.</t>
+  </si>
+  <si>
+    <t>4D7FDDB2-A708-46D3-A648-6C3B6AA45512</t>
+  </si>
+  <si>
+    <t>🙏🏻</t>
+  </si>
+  <si>
+    <t>Spirituality &amp; Mysticism</t>
+  </si>
+  <si>
+    <t>Discuss the concept of the Akashic Records and their significance in various mystical traditions.</t>
+  </si>
+  <si>
+    <t>8C19CC53-5332-4BF4-8AD0-E86CE8F1F7BB</t>
+  </si>
+  <si>
+    <t>Explore the role of sacred geometry in understanding the nature of the universe and its connection to spirituality.</t>
+  </si>
+  <si>
+    <t>50358192-08EC-4AB2-AFB4-686D5EAC94E8</t>
+  </si>
+  <si>
+    <t>Explain the concept of spiritual ascension and the stages one might experience during this journey.</t>
+  </si>
+  <si>
+    <t>EC14C9CF-40B7-4401-8C3C-45E41EEB5479</t>
+  </si>
+  <si>
+    <t>Analyze the symbolism and significance of the Tree of Life in different mystical traditions, including Kabbalah.</t>
+  </si>
+  <si>
+    <t>BB3225A0-9D44-4D8D-B05D-FE64E94C999C</t>
+  </si>
+  <si>
+    <t>Discuss the role of spirit guides in personal spiritual development and how one might connect with them.</t>
+  </si>
+  <si>
+    <t>85A9039D-FA31-4B6C-A727-D5C884222FFF</t>
+  </si>
+  <si>
+    <t>Explore the concept of astral projection and its implications for understanding consciousness beyond the physical body.</t>
+  </si>
+  <si>
+    <t>DF8C32B7-C01F-4B16-94F3-89FA266237FA</t>
+  </si>
+  <si>
+    <t>Analyze the role of the shadow self in spiritual growth and how embracing it can lead to personal transformation.</t>
+  </si>
+  <si>
+    <t>3E221F28-B96B-4553-B0FF-DE6EF8A33FB0</t>
+  </si>
+  <si>
+    <t>Discuss the significance of the third eye in various mystical traditions and its connection to higher consciousness.</t>
+  </si>
+  <si>
+    <t>5DA82E08-562D-4C37-82B0-DE7AF000132F</t>
+  </si>
+  <si>
+    <t>Explain the concept of divine timing and how it influences spiritual experiences and life events.</t>
+  </si>
+  <si>
+    <t>DC48DFEB-09CB-4816-82BD-05FD28EB33EC</t>
+  </si>
+  <si>
+    <t>Explore the role of alchemy in spiritual transformation and its symbolic significance in the pursuit of enlightenment.</t>
+  </si>
+  <si>
+    <t>46962558-485D-4CEA-930A-CEE9666E7785</t>
+  </si>
+  <si>
+    <t>🧘</t>
+  </si>
+  <si>
+    <t>What is the "Mountains and Waters Sutra"?</t>
   </si>
 </sst>
 </file>
@@ -10570,11 +11173,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCD347A-1D2E-BC47-8D31-C7D5B7396B53}">
-  <dimension ref="A1:I743"/>
+  <dimension ref="A1:I834"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A718" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E728" sqref="E728"/>
+      <pane ySplit="1" topLeftCell="A807" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H834" sqref="H834"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23626,6 +24229,1280 @@
         <v>1989</v>
       </c>
     </row>
+    <row r="744" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A744" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B744" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C744" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F744" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="745" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A745" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B745" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C745" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F745" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="746" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A746" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B746" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C746" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F746" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="747" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A747" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B747" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C747" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F747" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="748" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A748" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B748" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C748" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F748" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="749" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A749" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B749" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C749" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F749" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="750" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A750" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B750" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C750" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F750" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="751" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A751" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B751" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C751" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F751" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="752" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A752" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B752" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C752" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F752" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A753" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B753" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C753" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F753" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="754" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A754" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B754" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C754" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F754" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A755" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B755" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C755" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F755" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="756" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A756" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B756" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C756" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F756" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="757" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A757" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B757" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C757" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F757" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="758" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A758" t="s">
+        <v>2032</v>
+      </c>
+      <c r="B758" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C758" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F758" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="759" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A759" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B759" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C759" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F759" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A760" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B760" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C760" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F760" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A761" t="s">
+        <v>2038</v>
+      </c>
+      <c r="B761" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C761" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F761" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A762" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B762" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C762" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F762" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A763" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B763" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C763" t="s">
+        <v>2024</v>
+      </c>
+      <c r="F763" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="764" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A764" t="s">
+        <v>2044</v>
+      </c>
+      <c r="B764" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C764" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F764" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="765" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A765" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B765" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C765" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F765" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="766" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A766" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B766" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C766" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F766" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="767" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A767" t="s">
+        <v>2052</v>
+      </c>
+      <c r="B767" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C767" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F767" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="768" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A768" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B768" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C768" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F768" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="769" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A769" t="s">
+        <v>2056</v>
+      </c>
+      <c r="B769" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C769" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F769" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="770" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A770" t="s">
+        <v>2058</v>
+      </c>
+      <c r="B770" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C770" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F770" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="771" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A771" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B771" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C771" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F771" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A772" t="s">
+        <v>2062</v>
+      </c>
+      <c r="B772" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C772" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F772" t="s">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="773" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A773" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B773" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C773" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F773" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="774" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A774" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B774" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C774" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F774" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="775" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A775" t="s">
+        <v>2070</v>
+      </c>
+      <c r="B775" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C775" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F775" t="s">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="776" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A776" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B776" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C776" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F776" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="777" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A777" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B777" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C777" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F777" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="778" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A778" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B778" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C778" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F778" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="779" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A779" t="s">
+        <v>2078</v>
+      </c>
+      <c r="B779" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C779" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F779" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="780" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A780" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B780" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C780" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F780" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="781" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A781" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B781" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C781" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F781" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="782" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A782" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B782" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C782" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F782" t="s">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="783" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A783" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B783" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C783" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F783" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="784" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A784" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B784" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C784" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F784" t="s">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="785" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A785" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B785" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C785" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F785" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="786" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A786" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B786" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C786" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F786" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="787" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A787" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B787" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C787" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F787" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="788" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A788" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B788" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C788" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F788" t="s">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="789" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A789" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B789" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C789" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F789" t="s">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="790" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A790" t="s">
+        <v>2102</v>
+      </c>
+      <c r="B790" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C790" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F790" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="791" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A791" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B791" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C791" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F791" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="792" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A792" t="s">
+        <v>2106</v>
+      </c>
+      <c r="B792" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C792" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F792" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="793" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A793" t="s">
+        <v>2108</v>
+      </c>
+      <c r="B793" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C793" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F793" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="794" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A794" t="s">
+        <v>2110</v>
+      </c>
+      <c r="B794" t="s">
+        <v>2111</v>
+      </c>
+      <c r="C794" t="s">
+        <v>2112</v>
+      </c>
+      <c r="F794" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="795" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A795" t="s">
+        <v>2114</v>
+      </c>
+      <c r="B795" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C795" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F795" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="796" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A796" t="s">
+        <v>2116</v>
+      </c>
+      <c r="B796" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C796" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F796" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="797" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A797" t="s">
+        <v>2118</v>
+      </c>
+      <c r="B797" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C797" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F797" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="798" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A798" t="s">
+        <v>2120</v>
+      </c>
+      <c r="B798" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C798" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F798" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="799" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A799" t="s">
+        <v>2122</v>
+      </c>
+      <c r="B799" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C799" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F799" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="800" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A800" t="s">
+        <v>2124</v>
+      </c>
+      <c r="B800" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C800" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F800" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="801" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A801" t="s">
+        <v>2126</v>
+      </c>
+      <c r="B801" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C801" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F801" t="s">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="802" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A802" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B802" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C802" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F802" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="803" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A803" t="s">
+        <v>2130</v>
+      </c>
+      <c r="B803" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C803" t="s">
+        <v>2090</v>
+      </c>
+      <c r="F803" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="804" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A804" t="s">
+        <v>2132</v>
+      </c>
+      <c r="B804" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C804" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F804" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="805" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A805" t="s">
+        <v>2136</v>
+      </c>
+      <c r="B805" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C805" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F805" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="806" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A806" s="1" t="s">
+        <v>2138</v>
+      </c>
+      <c r="B806" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C806" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F806" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="807" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A807" t="s">
+        <v>2140</v>
+      </c>
+      <c r="B807" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C807" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F807" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="808" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A808" t="s">
+        <v>2142</v>
+      </c>
+      <c r="B808" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C808" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F808" t="s">
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="809" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A809" t="s">
+        <v>2144</v>
+      </c>
+      <c r="B809" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C809" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F809" t="s">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="810" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A810" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B810" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C810" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F810" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="811" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A811" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B811" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C811" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F811" t="s">
+        <v>2149</v>
+      </c>
+    </row>
+    <row r="812" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A812" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B812" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C812" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F812" t="s">
+        <v>2151</v>
+      </c>
+    </row>
+    <row r="813" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A813" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B813" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C813" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F813" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="814" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A814" t="s">
+        <v>2154</v>
+      </c>
+      <c r="B814" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C814" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F814" t="s">
+        <v>2157</v>
+      </c>
+    </row>
+    <row r="815" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A815" t="s">
+        <v>2158</v>
+      </c>
+      <c r="B815" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C815" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F815" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="816" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A816" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B816" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C816" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F816" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="817" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A817" t="s">
+        <v>2162</v>
+      </c>
+      <c r="B817" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C817" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F817" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="818" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A818" t="s">
+        <v>2164</v>
+      </c>
+      <c r="B818" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C818" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F818" t="s">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="819" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A819" t="s">
+        <v>2166</v>
+      </c>
+      <c r="B819" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C819" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F819" t="s">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="820" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A820" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B820" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C820" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F820" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="821" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A821" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B821" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C821" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F821" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="822" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A822" t="s">
+        <v>2172</v>
+      </c>
+      <c r="B822" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C822" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F822" t="s">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="823" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A823" t="s">
+        <v>2174</v>
+      </c>
+      <c r="B823" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C823" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F823" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="824" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A824" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B824" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C824" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F824" t="s">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="825" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A825" t="s">
+        <v>2180</v>
+      </c>
+      <c r="B825" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C825" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F825" t="s">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="826" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A826" t="s">
+        <v>2182</v>
+      </c>
+      <c r="B826" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C826" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F826" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="827" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A827" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B827" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C827" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F827" t="s">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="828" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A828" t="s">
+        <v>2186</v>
+      </c>
+      <c r="B828" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C828" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F828" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="829" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A829" t="s">
+        <v>2188</v>
+      </c>
+      <c r="B829" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C829" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F829" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="830" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A830" t="s">
+        <v>2190</v>
+      </c>
+      <c r="B830" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C830" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F830" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="831" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A831" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B831" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C831" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F831" t="s">
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="832" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A832" t="s">
+        <v>2194</v>
+      </c>
+      <c r="B832" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C832" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F832" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="833" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A833" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B833" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C833" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F833" t="s">
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="834" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A834" t="s">
+        <v>2198</v>
+      </c>
+      <c r="B834" t="s">
+        <v>2199</v>
+      </c>
+      <c r="C834" t="s">
+        <v>226</v>
+      </c>
+      <c r="F834" t="s">
+        <v>2200</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I713" xr:uid="{2D1BFCA3-AD4D-7945-98F5-2EB6B38B5422}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>